<commit_message>
Updated User Story Maps and  USM Backlog
</commit_message>
<xml_diff>
--- a/Documentation/URStreamSight USM Backlog.xlsx
+++ b/Documentation/URStreamSight USM Backlog.xlsx
@@ -35,7 +35,7 @@
         </d:r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B19" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -46,7 +46,7 @@
         </d:r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0">
+    <comment ref="B30" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -57,7 +57,7 @@
         </d:r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0">
+    <comment ref="B36" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Activity</t>
   </si>
@@ -136,42 +136,63 @@
     <t>Hifi prototype of web app</t>
   </si>
   <si>
+    <t>Release 0.3 MVP</t>
+  </si>
+  <si>
+    <t>Continue Architecture Research</t>
+  </si>
+  <si>
+    <t>Update USM</t>
+  </si>
+  <si>
+    <t>Release 1 MVP</t>
+  </si>
+  <si>
+    <t>Setup CICD for front end</t>
+  </si>
+  <si>
+    <t>Create Web App Project</t>
+  </si>
+  <si>
+    <t>Install necessary libraries</t>
+  </si>
+  <si>
+    <t>Add Login Page</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Release 2 MVP</t>
+  </si>
+  <si>
+    <t>Create API Endpoints</t>
+  </si>
+  <si>
     <t>Doing</t>
   </si>
   <si>
-    <t>Release 0.3 MVP</t>
-  </si>
-  <si>
-    <t>Continue Architecture Research</t>
-  </si>
-  <si>
-    <t>Update USM</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Release 1 MVP</t>
-  </si>
-  <si>
-    <t>Create Web App Project</t>
-  </si>
-  <si>
-    <t>Install necessary libraries</t>
-  </si>
-  <si>
-    <t>Add Login Page</t>
-  </si>
-  <si>
     <t>Tie in API calls and database storage</t>
   </si>
   <si>
-    <t>Release 2 MVP</t>
+    <t>Update CICD pipeline</t>
+  </si>
+  <si>
+    <t>Add additional API endpoints</t>
+  </si>
+  <si>
+    <t>Release 3 MVP</t>
   </si>
   <si>
     <t>Add Login Functionality</t>
   </si>
   <si>
+    <t>Add Test and Staging server to CICD pipeline</t>
+  </si>
+  <si>
+    <t>Release 4 Future Release MVP</t>
+  </si>
+  <si>
     <t>Neighbourhood Recycling Data</t>
   </si>
   <si>
@@ -208,9 +229,6 @@
     <t>Add Zoom Function</t>
   </si>
   <si>
-    <t>Release 3 MVP</t>
-  </si>
-  <si>
     <t>Add tool tip on hover</t>
   </si>
   <si>
@@ -271,7 +289,25 @@
     <t>Is archived</t>
   </si>
   <si>
+    <t>9/14/2020 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>10/5/2020 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>11/2/2020 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>11/16/2020 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>11/30/2020 12:00:00 AM</t>
   </si>
   <si>
     <t>Persona</t>
@@ -362,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="1"/>
   </sheetViews>
@@ -374,7 +410,7 @@
     <col min="4" max="4" width="80" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="13.0257917131696" customWidth="1"/>
-    <col min="7" max="7" width="16.0732236589704" customWidth="1"/>
+    <col min="7" max="7" width="27.9847739083426" customWidth="1"/>
     <col min="8" max="16384" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -514,11 +550,11 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>14</v>
@@ -532,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>11</v>
@@ -542,7 +578,7 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>14</v>
@@ -556,17 +592,17 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>14</v>
@@ -580,17 +616,17 @@
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>14</v>
@@ -604,17 +640,17 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>14</v>
@@ -628,17 +664,17 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>14</v>
@@ -652,17 +688,17 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>14</v>
@@ -676,17 +712,17 @@
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>14</v>
@@ -694,23 +730,23 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>14</v>
@@ -718,23 +754,23 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>14</v>
@@ -742,23 +778,23 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>14</v>
@@ -766,23 +802,23 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>14</v>
@@ -790,23 +826,23 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>14</v>
@@ -814,23 +850,23 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>14</v>
@@ -838,23 +874,23 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>14</v>
@@ -862,23 +898,23 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>14</v>
@@ -886,23 +922,23 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>14</v>
@@ -910,23 +946,23 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>14</v>
@@ -934,23 +970,23 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>14</v>
@@ -958,13 +994,13 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>11</v>
@@ -974,21 +1010,21 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>11</v>
@@ -998,90 +1034,90 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>54</v>
@@ -1090,22 +1126,22 @@
         <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>56</v>
@@ -1114,22 +1150,22 @@
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>57</v>
@@ -1138,22 +1174,22 @@
         <v>11</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>58</v>
@@ -1162,14 +1198,134 @@
         <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1337,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="1"/>
   </sheetViews>
@@ -1198,22 +1354,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
@@ -1222,16 +1378,16 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
@@ -1240,75 +1396,75 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -1318,10 +1474,28 @@
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1347,44 +1521,44 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional documentation and updated USM
Added additional project documentation and updated the USM and backlog
</commit_message>
<xml_diff>
--- a/Documentation/URStreamSight USM Backlog.xlsx
+++ b/Documentation/URStreamSight USM Backlog.xlsx
@@ -35,7 +35,7 @@
         </d:r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0">
+    <comment ref="B24" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -46,7 +46,7 @@
         </d:r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0">
+    <comment ref="B42" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -57,7 +57,7 @@
         </d:r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0">
+    <comment ref="B53" authorId="0">
       <text>
         <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
           <rPr>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>Activity</t>
   </si>
@@ -178,22 +178,40 @@
     <t>Add additional API endpoints</t>
   </si>
   <si>
+    <t>Review API Implementation</t>
+  </si>
+  <si>
+    <t>Release 4 MVP (Feb 4)</t>
+  </si>
+  <si>
+    <t>Add additional API Endpoints</t>
+  </si>
+  <si>
+    <t>Add API calls to Frontend</t>
+  </si>
+  <si>
+    <t>Release 5 MVP (Feb 25)</t>
+  </si>
+  <si>
+    <t>Research Front end Integrations</t>
+  </si>
+  <si>
+    <t>Add Login Functionality</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Release 6 MVP (Mar 4)</t>
+  </si>
+  <si>
+    <t>Add Test and Staging server to CICD pipeline</t>
+  </si>
+  <si>
     <t>Add Login Page</t>
   </si>
   <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Release 4 Future Release MVP</t>
-  </si>
-  <si>
-    <t>Add Login Functionality</t>
-  </si>
-  <si>
-    <t>Add Test and Staging server to CICD pipeline</t>
-  </si>
-  <si>
-    <t>Release 5</t>
+    <t>Release 7 MVP</t>
   </si>
   <si>
     <t>Neighbourhood Recycling Data</t>
@@ -238,15 +256,24 @@
     <t>Start to add RBAC</t>
   </si>
   <si>
+    <t>Finish RBAC implementation</t>
+  </si>
+  <si>
+    <t>Add basic tests</t>
+  </si>
+  <si>
+    <t>Create documentation for new front end pages</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>Add Testing to CICD Pipeline</t>
+  </si>
+  <si>
     <t>Implement Testing Plan</t>
   </si>
   <si>
-    <t>Add Testing to CICD Pipeline</t>
-  </si>
-  <si>
-    <t>Add heat map of contaminant disposal</t>
-  </si>
-  <si>
     <t>Add tool tip on hover</t>
   </si>
   <si>
@@ -277,12 +304,18 @@
     <t>Research Testing plan Options</t>
   </si>
   <si>
-    <t>Doing</t>
+    <t>Verify Database seeding</t>
+  </si>
+  <si>
+    <t>Add basic heat map of contaminant disposal</t>
   </si>
   <si>
     <t>Add Test Coverage to CICD Pipeline</t>
   </si>
   <si>
+    <t>Add additional API calls in front end</t>
+  </si>
+  <si>
     <t>Add Export Function</t>
   </si>
   <si>
@@ -353,6 +386,12 @@
   </si>
   <si>
     <t>2/4/2021 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>2/5/2021 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>2/25/2021 12:00:00 AM</t>
   </si>
   <si>
     <t>Persona</t>
@@ -443,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="1"/>
   </sheetViews>
@@ -451,7 +490,7 @@
   <cols>
     <col min="1" max="1" width="28.5055127825056" customWidth="1"/>
     <col min="2" max="2" width="47.4342694963728" customWidth="1"/>
-    <col min="3" max="3" width="40.5797293526786" customWidth="1"/>
+    <col min="3" max="3" width="42.7905752999442" customWidth="1"/>
     <col min="4" max="4" width="80" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="13.0257917131696" customWidth="1"/>
@@ -859,11 +898,11 @@
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>14</v>
@@ -877,17 +916,17 @@
         <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>14</v>
@@ -901,17 +940,17 @@
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>14</v>
@@ -919,13 +958,13 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>11</v>
@@ -935,7 +974,7 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>14</v>
@@ -943,23 +982,23 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>14</v>
@@ -967,23 +1006,23 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>14</v>
@@ -991,23 +1030,23 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>14</v>
@@ -1015,13 +1054,13 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>11</v>
@@ -1031,7 +1070,7 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>14</v>
@@ -1039,13 +1078,13 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>11</v>
@@ -1055,7 +1094,7 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>14</v>
@@ -1063,13 +1102,13 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>11</v>
@@ -1079,7 +1118,7 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>14</v>
@@ -1087,13 +1126,13 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>11</v>
@@ -1103,7 +1142,7 @@
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>14</v>
@@ -1111,13 +1150,13 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>11</v>
@@ -1127,7 +1166,7 @@
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>14</v>
@@ -1135,13 +1174,13 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>11</v>
@@ -1151,7 +1190,7 @@
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>14</v>
@@ -1159,13 +1198,13 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>11</v>
@@ -1175,7 +1214,7 @@
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>14</v>
@@ -1183,13 +1222,13 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>11</v>
@@ -1199,7 +1238,7 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>14</v>
@@ -1207,23 +1246,23 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>14</v>
@@ -1231,23 +1270,23 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>14</v>
@@ -1255,23 +1294,23 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>14</v>
@@ -1279,23 +1318,23 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>14</v>
@@ -1303,10 +1342,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>60</v>
@@ -1319,21 +1358,21 @@
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>11</v>
@@ -1343,42 +1382,42 @@
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>64</v>
@@ -1387,22 +1426,22 @@
         <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>65</v>
@@ -1411,22 +1450,22 @@
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>66</v>
@@ -1435,73 +1474,73 @@
         <v>11</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>11</v>
@@ -1511,21 +1550,21 @@
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>11</v>
@@ -1535,63 +1574,279 @@
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="2"/>
+      <c r="D47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="3"/>
+      <c r="G47" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="2"/>
+      <c r="D48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="3"/>
+      <c r="G48" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
@@ -1602,7 +1857,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="1"/>
   </sheetViews>
@@ -1619,22 +1874,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
@@ -1643,16 +1898,16 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3">
@@ -1661,16 +1916,16 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
@@ -1679,16 +1934,16 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5">
@@ -1697,16 +1952,16 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6">
@@ -1715,16 +1970,16 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
@@ -1733,52 +1988,88 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1804,44 +2095,44 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>